<commit_message>
Updated Vikash's section on the master document
</commit_message>
<xml_diff>
--- a/Deliverables/Understanding Data/NYBG/Inventory Data/NYBG_Species Code_Master List_JAS12022016.xlsx
+++ b/Deliverables/Understanding Data/NYBG/Inventory Data/NYBG_Species Code_Master List_JAS12022016.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikash Kumar\OneDrive\UNOmaha\Study\Sem 3\ISQA 8086 - 2\NY Botanical Garden\1 - Work\DataSnipers\Deliverables\Understanding Data\NYBG\Inventory Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_E59C6CBCFA620360A947A80FF1535EC7D573F297" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{81AD8EE3-0133-4988-94FF-2633B4E539BD}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_E59C6CBCFA620360A947A80FF1535EC7D573F297" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{2653DA01-00D5-41DC-A892-47C5B06E17E4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12900" windowHeight="6330" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,10 +17,10 @@
     <sheet name="pre-2016 Codes (need reconciled" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master Spp. List (woody + herb)'!$A$1:$D$160</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master Spp. List (woody + herb)'!$A$1:$F$160</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'pre-2016 Codes (need reconciled'!$A$1:$F$96</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1876,7 +1876,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F6"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3751,11 +3751,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D160" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState ref="A2:E157">
-      <sortCondition ref="B1:B157"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:F160" xr:uid="{5134C2F8-3BF2-4E6A-9338-3B6CFC40769D}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -3771,7 +3767,7 @@
   <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>